<commit_message>
HTML divided into React components
</commit_message>
<xml_diff>
--- a/dedication.xlsx
+++ b/dedication.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t xml:space="preserve">Dedication code </t>
   </si>
@@ -38,13 +38,16 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>asdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +58,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,12 +97,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -398,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,59 +424,101 @@
     <col min="2" max="2" width="26.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="3">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="3">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="3">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="3">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="3">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3">
         <v>8</v>
       </c>
     </row>

</xml_diff>